<commit_message>
Updated ENG-GER match files
more corrections to substitutions
</commit_message>
<xml_diff>
--- a/source/excel/shebelieves-cup-2016/shebelieves-cup-2016-eng-ger-030616.xlsx
+++ b/source/excel/shebelieves-cup-2016/shebelieves-cup-2016-eng-ger-030616.xlsx
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1106" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E1138" sqref="E1138"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>